<commit_message>
Esta versión fue entregada a la profa el 10/12/2024.
</commit_message>
<xml_diff>
--- a/Gestion_de_Cursos/Archivos_exportados/2024/2-2024/listas_asistencia/lista_asistencia_Taller_de_sueldos_y_salarios.xlsx
+++ b/Gestion_de_Cursos/Archivos_exportados/2024/2-2024/listas_asistencia/lista_asistencia_Taller_de_sueldos_y_salarios.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <workbookPr/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\andyb\Documents\NetBeansProjects\nuevo\DesarrolloAcademicoIntegrado\Gestion_de_Cursos\Archivos_importados\2024\2-2024\formato_de_listas_de_asistencia\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ACFB02F-0341-4091-8921-8C565FE8A1AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7755"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="lista de asistencia" sheetId="1" r:id="rId1"/>
@@ -23,10 +24,21 @@
     <definedName name="Nombre_del_Curso">[1]cursos!$C$2:$C$97</definedName>
     <definedName name="x_nombre">'[1]plantilla de personal'!$D$2:$D$365</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -215,7 +227,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
   <fonts count="13" x14ac:knownFonts="1">
     <font>
@@ -773,47 +785,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="118">
+  <cellXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="20" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -831,25 +831,25 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -864,22 +864,22 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="29" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="32" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -888,78 +888,62 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1000,10 +984,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1021,7 +1002,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1078,10 +1059,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1090,39 +1071,40 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="6" fillId="0" borderId="34" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="5" fillId="0" borderId="34" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2 2" xfId="1"/>
+    <cellStyle name="Normal 2 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1132,11 +1114,6 @@
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -1220,7 +1197,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="result para registrar"/>
@@ -3883,1114 +3860,1055 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Hoja1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:T42"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showOutlineSymbols="0" view="pageBreakPreview" topLeftCell="A5" zoomScale="87" zoomScaleNormal="62" zoomScaleSheetLayoutView="87" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView showGridLines="0" tabSelected="1" showOutlineSymbols="0" view="pageBreakPreview" topLeftCell="A24" zoomScale="104" zoomScaleNormal="62" zoomScaleSheetLayoutView="62" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8:S8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="2" width="6.7109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="2" width="11.5703125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="2" width="14.85546875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="2" width="10.140625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="46" width="19.85546875" collapsed="true"/>
-    <col min="6" max="9" customWidth="true" style="2" width="12.42578125" collapsed="true"/>
-    <col min="10" max="11" customWidth="true" style="2" width="4.42578125" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" style="2" width="3.7109375" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" style="2" width="4.5703125" collapsed="true"/>
-    <col min="14" max="18" customWidth="true" style="2" width="4.0" collapsed="true"/>
-    <col min="19" max="19" customWidth="true" style="2" width="5.0" collapsed="true"/>
-    <col min="20" max="20" customWidth="true" style="2" width="15.140625" collapsed="true"/>
-    <col min="21" max="16384" style="2" width="11.42578125" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" style="1" width="6.6640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="11.5546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="14.88671875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="10.109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="3" width="19.88671875" collapsed="true"/>
+    <col min="6" max="9" customWidth="true" style="1" width="12.44140625" collapsed="true"/>
+    <col min="10" max="11" customWidth="true" style="1" width="4.44140625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="1" width="3.6640625" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" style="1" width="4.5546875" collapsed="true"/>
+    <col min="14" max="18" customWidth="true" style="1" width="4.0" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" style="1" width="5.0" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" style="1" width="15.109375" collapsed="true"/>
+    <col min="21" max="16384" style="1" width="11.44140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="96"/>
-      <c r="D1" s="99" t="s">
+    <row r="1" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C1" s="83"/>
+      <c r="D1" s="86" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="100"/>
-      <c r="F1" s="100"/>
-      <c r="G1" s="100"/>
-      <c r="H1" s="100"/>
-      <c r="I1" s="101"/>
-      <c r="J1" s="99" t="s">
+      <c r="E1" s="87"/>
+      <c r="F1" s="87"/>
+      <c r="G1" s="87"/>
+      <c r="H1" s="87"/>
+      <c r="I1" s="88"/>
+      <c r="J1" s="86" t="s">
         <v>1</v>
       </c>
-      <c r="K1" s="100"/>
-      <c r="L1" s="100"/>
-      <c r="M1" s="100"/>
-      <c r="N1" s="100"/>
-      <c r="O1" s="100"/>
-      <c r="P1" s="100"/>
-      <c r="Q1" s="100"/>
-      <c r="R1" s="100"/>
-      <c r="S1" s="101"/>
+      <c r="K1" s="87"/>
+      <c r="L1" s="87"/>
+      <c r="M1" s="87"/>
+      <c r="N1" s="87"/>
+      <c r="O1" s="87"/>
+      <c r="P1" s="87"/>
+      <c r="Q1" s="87"/>
+      <c r="R1" s="87"/>
+      <c r="S1" s="88"/>
     </row>
-    <row r="2" spans="1:20" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="97"/>
-      <c r="D2" s="102"/>
-      <c r="E2" s="103"/>
-      <c r="F2" s="103"/>
-      <c r="G2" s="103"/>
-      <c r="H2" s="103"/>
-      <c r="I2" s="104"/>
-      <c r="J2" s="102"/>
-      <c r="K2" s="103"/>
-      <c r="L2" s="103"/>
-      <c r="M2" s="103"/>
-      <c r="N2" s="103"/>
-      <c r="O2" s="103"/>
-      <c r="P2" s="103"/>
-      <c r="Q2" s="103"/>
-      <c r="R2" s="103"/>
-      <c r="S2" s="104"/>
+    <row r="2" spans="1:20" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="84"/>
+      <c r="D2" s="89"/>
+      <c r="E2" s="90"/>
+      <c r="F2" s="90"/>
+      <c r="G2" s="90"/>
+      <c r="H2" s="90"/>
+      <c r="I2" s="91"/>
+      <c r="J2" s="89"/>
+      <c r="K2" s="90"/>
+      <c r="L2" s="90"/>
+      <c r="M2" s="90"/>
+      <c r="N2" s="90"/>
+      <c r="O2" s="90"/>
+      <c r="P2" s="90"/>
+      <c r="Q2" s="90"/>
+      <c r="R2" s="90"/>
+      <c r="S2" s="91"/>
     </row>
-    <row r="3" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="97"/>
-      <c r="D3" s="99" t="s">
+    <row r="3" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C3" s="84"/>
+      <c r="D3" s="86" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="100"/>
-      <c r="F3" s="100"/>
-      <c r="G3" s="100"/>
-      <c r="H3" s="100"/>
-      <c r="I3" s="101"/>
-      <c r="J3" s="105" t="s">
+      <c r="E3" s="87"/>
+      <c r="F3" s="87"/>
+      <c r="G3" s="87"/>
+      <c r="H3" s="87"/>
+      <c r="I3" s="88"/>
+      <c r="J3" s="92" t="s">
         <v>3</v>
       </c>
-      <c r="K3" s="106"/>
-      <c r="L3" s="106"/>
-      <c r="M3" s="106"/>
-      <c r="N3" s="107">
+      <c r="K3" s="93"/>
+      <c r="L3" s="93"/>
+      <c r="M3" s="93"/>
+      <c r="N3" s="94">
         <v>1</v>
       </c>
-      <c r="O3" s="107" t="s">
+      <c r="O3" s="94" t="s">
         <v>4</v>
       </c>
-      <c r="P3" s="106">
+      <c r="P3" s="93">
         <v>1</v>
       </c>
-      <c r="Q3" s="106"/>
-      <c r="R3" s="106"/>
-      <c r="S3" s="109"/>
+      <c r="Q3" s="93"/>
+      <c r="R3" s="93"/>
+      <c r="S3" s="96"/>
     </row>
-    <row r="4" spans="1:20" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="98"/>
-      <c r="D4" s="102"/>
-      <c r="E4" s="103"/>
-      <c r="F4" s="103"/>
-      <c r="G4" s="103"/>
-      <c r="H4" s="103"/>
-      <c r="I4" s="104"/>
-      <c r="J4" s="102"/>
-      <c r="K4" s="103"/>
-      <c r="L4" s="103"/>
-      <c r="M4" s="103"/>
-      <c r="N4" s="108"/>
-      <c r="O4" s="108"/>
-      <c r="P4" s="103"/>
-      <c r="Q4" s="103"/>
-      <c r="R4" s="103"/>
-      <c r="S4" s="104"/>
+    <row r="4" spans="1:20" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C4" s="85"/>
+      <c r="D4" s="89"/>
+      <c r="E4" s="90"/>
+      <c r="F4" s="90"/>
+      <c r="G4" s="90"/>
+      <c r="H4" s="90"/>
+      <c r="I4" s="91"/>
+      <c r="J4" s="89"/>
+      <c r="K4" s="90"/>
+      <c r="L4" s="90"/>
+      <c r="M4" s="90"/>
+      <c r="N4" s="95"/>
+      <c r="O4" s="95"/>
+      <c r="P4" s="90"/>
+      <c r="Q4" s="90"/>
+      <c r="R4" s="90"/>
+      <c r="S4" s="91"/>
     </row>
-    <row r="5" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
-      <c r="O5" s="4"/>
-      <c r="P5" s="4"/>
-      <c r="Q5" s="4"/>
-      <c r="R5" s="4"/>
+    <row r="5" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D5" s="2"/>
     </row>
-    <row r="6" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="110" t="s">
+    <row r="6" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="97" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="110"/>
-      <c r="D6" s="110"/>
-      <c r="E6" s="110"/>
-      <c r="F6" s="110"/>
-      <c r="G6" s="110"/>
-      <c r="H6" s="110"/>
-      <c r="I6" s="110"/>
-      <c r="J6" s="110"/>
-      <c r="K6" s="110"/>
-      <c r="L6" s="110"/>
-      <c r="M6" s="110"/>
-      <c r="N6" s="110"/>
-      <c r="O6" s="110"/>
-      <c r="P6" s="110"/>
-      <c r="Q6" s="110"/>
-      <c r="R6" s="110"/>
+      <c r="C6" s="97"/>
+      <c r="D6" s="97"/>
+      <c r="E6" s="97"/>
+      <c r="F6" s="97"/>
+      <c r="G6" s="97"/>
+      <c r="H6" s="97"/>
+      <c r="I6" s="97"/>
+      <c r="J6" s="97"/>
+      <c r="K6" s="97"/>
+      <c r="L6" s="97"/>
+      <c r="M6" s="97"/>
+      <c r="N6" s="97"/>
+      <c r="O6" s="97"/>
+      <c r="P6" s="97"/>
+      <c r="Q6" s="97"/>
+      <c r="R6" s="97"/>
     </row>
-    <row r="7" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="e">
+    <row r="7" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="e">
         <f>CONCATENATE("CURSO NÚMERO: ",#REF!)</f>
         <v>#REF!</v>
       </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
-      <c r="N7" s="7"/>
-      <c r="O7" s="7"/>
-      <c r="P7" s="7"/>
-      <c r="Q7" s="7"/>
-      <c r="R7" s="7"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+      <c r="O7" s="4"/>
+      <c r="P7" s="4"/>
+      <c r="Q7" s="4"/>
+      <c r="R7" s="4"/>
     </row>
-    <row r="8" spans="1:20" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="9" t="s">
+    <row r="8" spans="1:20" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="111" t="s">
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="101" t="s">
         <v>34</v>
       </c>
-      <c r="E8" s="111"/>
-      <c r="F8" s="111"/>
-      <c r="G8" s="111"/>
-      <c r="H8" s="111"/>
-      <c r="I8" s="111"/>
-      <c r="J8" s="111"/>
-      <c r="K8" s="111"/>
-      <c r="L8" s="112"/>
-      <c r="M8" s="112"/>
-      <c r="N8" s="111"/>
-      <c r="O8" s="111"/>
-      <c r="P8" s="111"/>
-      <c r="Q8" s="111"/>
-      <c r="R8" s="111"/>
-      <c r="S8" s="111"/>
+      <c r="E8" s="101"/>
+      <c r="F8" s="101"/>
+      <c r="G8" s="101"/>
+      <c r="H8" s="101"/>
+      <c r="I8" s="101"/>
+      <c r="J8" s="101"/>
+      <c r="K8" s="101"/>
+      <c r="L8" s="101"/>
+      <c r="M8" s="101"/>
+      <c r="N8" s="101"/>
+      <c r="O8" s="101"/>
+      <c r="P8" s="101"/>
+      <c r="Q8" s="101"/>
+      <c r="R8" s="101"/>
+      <c r="S8" s="101"/>
     </row>
-    <row r="9" spans="1:20" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="113" t="s">
+    <row r="9" spans="1:20" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="98" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="113"/>
-      <c r="C9" s="113"/>
-      <c r="D9" s="114" t="s">
+      <c r="B9" s="98"/>
+      <c r="C9" s="98"/>
+      <c r="D9" s="101" t="s">
         <v>35</v>
       </c>
-      <c r="E9" s="114"/>
-      <c r="F9" s="114"/>
-      <c r="G9" s="114"/>
-      <c r="H9" s="114"/>
-      <c r="I9" s="11" t="s">
+      <c r="E9" s="101"/>
+      <c r="F9" s="101"/>
+      <c r="G9" s="101"/>
+      <c r="H9" s="101"/>
+      <c r="I9" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="J9" s="116" t="s">
+      <c r="J9" s="104" t="s">
         <v>39</v>
       </c>
-      <c r="K9" s="116"/>
-      <c r="L9" s="116"/>
-      <c r="M9" s="13"/>
-      <c r="N9" s="11" t="s">
+      <c r="K9" s="104"/>
+      <c r="L9" s="104"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="P9" s="12"/>
-      <c r="Q9" s="115" t="s">
+      <c r="P9" s="7"/>
+      <c r="Q9" s="105" t="s">
         <v>38</v>
       </c>
-      <c r="R9" s="115"/>
-      <c r="S9" s="115"/>
-      <c r="T9" s="115"/>
+      <c r="R9" s="105"/>
+      <c r="S9" s="105"/>
+      <c r="T9" s="105"/>
     </row>
-    <row r="10" spans="1:20" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="10" t="s">
+    <row r="10" spans="1:20" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="14"/>
-      <c r="D10" s="80" t="s">
+      <c r="B10" s="3"/>
+      <c r="D10" s="102" t="s">
         <v>36</v>
       </c>
-      <c r="E10" s="80"/>
-      <c r="F10" s="80"/>
-      <c r="G10" s="80"/>
-      <c r="H10" s="80"/>
-      <c r="J10" s="15"/>
-      <c r="K10" s="54" t="s">
+      <c r="E10" s="102"/>
+      <c r="F10" s="102"/>
+      <c r="G10" s="102"/>
+      <c r="H10" s="102"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="100" t="s">
         <v>41</v>
       </c>
-      <c r="L10" s="54"/>
-      <c r="M10" s="54"/>
-      <c r="N10" s="54"/>
-      <c r="O10" s="54"/>
-      <c r="P10" s="54"/>
-      <c r="Q10" s="54"/>
-      <c r="R10" s="54"/>
+      <c r="L10" s="100"/>
+      <c r="M10" s="100"/>
+      <c r="N10" s="100"/>
+      <c r="O10" s="100"/>
+      <c r="P10" s="100"/>
+      <c r="Q10" s="100"/>
+      <c r="R10" s="100"/>
     </row>
-    <row r="11" spans="1:20" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="81" t="s">
+    <row r="11" spans="1:20" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="68" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="81"/>
-      <c r="D11" s="47" t="s">
+      <c r="B11" s="68"/>
+      <c r="D11" s="103" t="s">
         <v>37</v>
       </c>
-      <c r="E11" s="48"/>
-      <c r="F11" s="47"/>
-      <c r="G11" s="47"/>
-      <c r="H11" s="47"/>
-      <c r="I11" s="16"/>
-      <c r="J11" s="16"/>
-      <c r="K11" s="55" t="s">
+      <c r="E11" s="103"/>
+      <c r="F11" s="103"/>
+      <c r="G11" s="103"/>
+      <c r="H11" s="103"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="L11" s="55"/>
-      <c r="M11" s="55"/>
-      <c r="N11" s="55"/>
-      <c r="O11" s="55"/>
-      <c r="P11" s="55"/>
-      <c r="Q11" s="55"/>
-      <c r="R11" s="55"/>
+      <c r="L11" s="45"/>
+      <c r="M11" s="45"/>
+      <c r="N11" s="45"/>
+      <c r="O11" s="45"/>
+      <c r="P11" s="45"/>
+      <c r="Q11" s="45"/>
+      <c r="R11" s="45"/>
     </row>
-    <row r="12" spans="1:20" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="17"/>
-      <c r="I12" s="16"/>
-      <c r="J12" s="16"/>
-      <c r="K12" s="16"/>
-      <c r="L12" s="16"/>
-      <c r="M12" s="16"/>
-      <c r="N12" s="16"/>
-      <c r="O12" s="16"/>
-      <c r="P12" s="16"/>
-      <c r="Q12" s="4"/>
-      <c r="R12" s="4"/>
+    <row r="12" spans="1:20" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="10"/>
+      <c r="N12" s="10"/>
+      <c r="O12" s="10"/>
+      <c r="P12" s="10"/>
     </row>
-    <row r="13" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="70" t="s">
+    <row r="13" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="83" t="s">
+      <c r="B13" s="70" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="84"/>
-      <c r="D13" s="85"/>
-      <c r="E13" s="84" t="s">
+      <c r="C13" s="71"/>
+      <c r="D13" s="72"/>
+      <c r="E13" s="71" t="s">
         <v>14</v>
       </c>
-      <c r="F13" s="93" t="s">
+      <c r="F13" s="80" t="s">
         <v>15</v>
       </c>
-      <c r="G13" s="93"/>
-      <c r="H13" s="93"/>
-      <c r="I13" s="93"/>
-      <c r="J13" s="67" t="s">
+      <c r="G13" s="80"/>
+      <c r="H13" s="80"/>
+      <c r="I13" s="80"/>
+      <c r="J13" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="K13" s="67" t="s">
+      <c r="K13" s="55" t="s">
         <v>17</v>
       </c>
-      <c r="L13" s="70" t="s">
+      <c r="L13" s="58" t="s">
         <v>18</v>
       </c>
-      <c r="M13" s="71"/>
-      <c r="N13" s="72" t="s">
+      <c r="M13" s="59"/>
+      <c r="N13" s="60" t="s">
         <v>19</v>
       </c>
-      <c r="O13" s="72"/>
-      <c r="P13" s="72"/>
-      <c r="Q13" s="72"/>
-      <c r="R13" s="72"/>
-      <c r="S13" s="71"/>
-      <c r="T13" s="75" t="s">
+      <c r="O13" s="60"/>
+      <c r="P13" s="60"/>
+      <c r="Q13" s="60"/>
+      <c r="R13" s="60"/>
+      <c r="S13" s="59"/>
+      <c r="T13" s="63" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="78"/>
-      <c r="B14" s="86"/>
-      <c r="C14" s="87"/>
-      <c r="D14" s="88"/>
-      <c r="E14" s="87"/>
-      <c r="F14" s="94"/>
-      <c r="G14" s="94"/>
-      <c r="H14" s="94"/>
-      <c r="I14" s="94"/>
-      <c r="J14" s="68"/>
-      <c r="K14" s="68"/>
-      <c r="L14" s="78" t="s">
+    <row r="14" spans="1:20" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="66"/>
+      <c r="B14" s="73"/>
+      <c r="C14" s="74"/>
+      <c r="D14" s="75"/>
+      <c r="E14" s="74"/>
+      <c r="F14" s="81"/>
+      <c r="G14" s="81"/>
+      <c r="H14" s="81"/>
+      <c r="I14" s="81"/>
+      <c r="J14" s="56"/>
+      <c r="K14" s="56"/>
+      <c r="L14" s="66" t="s">
         <v>21</v>
       </c>
-      <c r="M14" s="79"/>
-      <c r="N14" s="73"/>
-      <c r="O14" s="73"/>
-      <c r="P14" s="73"/>
-      <c r="Q14" s="73"/>
-      <c r="R14" s="73"/>
-      <c r="S14" s="74"/>
-      <c r="T14" s="76"/>
+      <c r="M14" s="67"/>
+      <c r="N14" s="61"/>
+      <c r="O14" s="61"/>
+      <c r="P14" s="61"/>
+      <c r="Q14" s="61"/>
+      <c r="R14" s="61"/>
+      <c r="S14" s="62"/>
+      <c r="T14" s="64"/>
     </row>
-    <row r="15" spans="1:20" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="82"/>
-      <c r="B15" s="89"/>
-      <c r="C15" s="90"/>
-      <c r="D15" s="91"/>
-      <c r="E15" s="92"/>
-      <c r="F15" s="95"/>
-      <c r="G15" s="95"/>
-      <c r="H15" s="95"/>
-      <c r="I15" s="95"/>
-      <c r="J15" s="69"/>
-      <c r="K15" s="69"/>
-      <c r="L15" s="18" t="s">
+    <row r="15" spans="1:20" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="69"/>
+      <c r="B15" s="76"/>
+      <c r="C15" s="77"/>
+      <c r="D15" s="78"/>
+      <c r="E15" s="79"/>
+      <c r="F15" s="82"/>
+      <c r="G15" s="82"/>
+      <c r="H15" s="82"/>
+      <c r="I15" s="82"/>
+      <c r="J15" s="57"/>
+      <c r="K15" s="57"/>
+      <c r="L15" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="M15" s="18" t="s">
+      <c r="M15" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="N15" s="19" t="s">
+      <c r="N15" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="O15" s="20" t="s">
+      <c r="O15" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="P15" s="20" t="s">
+      <c r="P15" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="Q15" s="20" t="s">
+      <c r="Q15" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="R15" s="21" t="s">
+      <c r="R15" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="S15" s="22" t="s">
+      <c r="S15" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="T15" s="77"/>
+      <c r="T15" s="65"/>
     </row>
-    <row r="16" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" t="n" s="117">
+    <row r="16" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" t="n" s="106">
         <v>1.0</v>
       </c>
-      <c r="B16" t="s" s="117">
+      <c r="B16" t="s" s="106">
         <v>42</v>
       </c>
-      <c r="C16" s="56"/>
-      <c r="D16" s="56"/>
-      <c r="E16" t="s" s="117">
+      <c r="C16" s="46"/>
+      <c r="D16" s="46"/>
+      <c r="E16" t="s" s="106">
         <v>43</v>
       </c>
-      <c r="F16" t="s" s="117">
+      <c r="F16" t="s" s="106">
         <v>44</v>
       </c>
-      <c r="G16" s="58"/>
-      <c r="H16" s="58"/>
-      <c r="I16" s="59"/>
-      <c r="J16" t="s" s="117">
+      <c r="G16" s="48"/>
+      <c r="H16" s="48"/>
+      <c r="I16" s="49"/>
+      <c r="J16" t="s" s="106">
         <v>45</v>
       </c>
-      <c r="K16" t="s" s="117">
+      <c r="K16" t="s" s="106">
         <v>32</v>
       </c>
-      <c r="L16" t="s" s="117">
+      <c r="L16" t="s" s="106">
         <v>45</v>
       </c>
-      <c r="M16" t="s" s="117">
+      <c r="M16" t="s" s="106">
         <v>32</v>
       </c>
-      <c r="N16" s="28"/>
-      <c r="O16" s="29"/>
-      <c r="P16" s="28"/>
-      <c r="Q16" s="28"/>
-      <c r="R16" s="29"/>
-      <c r="S16" s="30"/>
-      <c r="T16" s="31"/>
+      <c r="N16" s="22"/>
+      <c r="O16" s="23"/>
+      <c r="P16" s="22"/>
+      <c r="Q16" s="22"/>
+      <c r="R16" s="23"/>
+      <c r="S16" s="24"/>
+      <c r="T16" s="25"/>
     </row>
-    <row r="17" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" t="n" s="117">
+    <row r="17" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" t="n" s="106">
         <v>2.0</v>
       </c>
-      <c r="B17" t="s" s="117">
+      <c r="B17" t="s" s="106">
         <v>46</v>
       </c>
-      <c r="C17" s="56"/>
-      <c r="D17" s="56"/>
-      <c r="E17" t="s" s="117">
+      <c r="C17" s="46"/>
+      <c r="D17" s="46"/>
+      <c r="E17" t="s" s="106">
         <v>47</v>
       </c>
-      <c r="F17" t="s" s="117">
+      <c r="F17" t="s" s="106">
         <v>48</v>
       </c>
-      <c r="G17" s="58"/>
-      <c r="H17" s="58"/>
-      <c r="I17" s="59"/>
-      <c r="J17" t="s" s="117">
+      <c r="G17" s="48"/>
+      <c r="H17" s="48"/>
+      <c r="I17" s="49"/>
+      <c r="J17" t="s" s="106">
         <v>32</v>
       </c>
-      <c r="K17" t="s" s="117">
+      <c r="K17" t="s" s="106">
         <v>45</v>
       </c>
-      <c r="L17" s="26"/>
-      <c r="M17" s="27"/>
-      <c r="N17" s="28"/>
-      <c r="O17" s="29"/>
-      <c r="P17" s="28"/>
-      <c r="Q17" s="28"/>
-      <c r="R17" s="29"/>
-      <c r="S17" s="32"/>
-      <c r="T17" s="33"/>
+      <c r="L17" s="20"/>
+      <c r="M17" s="21"/>
+      <c r="N17" s="22"/>
+      <c r="O17" s="23"/>
+      <c r="P17" s="22"/>
+      <c r="Q17" s="22"/>
+      <c r="R17" s="23"/>
+      <c r="S17" s="26"/>
+      <c r="T17" s="27"/>
     </row>
-    <row r="18" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" t="n" s="117">
+    <row r="18" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" t="n" s="106">
         <v>3.0</v>
       </c>
-      <c r="B18" t="s" s="117">
+      <c r="B18" t="s" s="106">
         <v>49</v>
       </c>
-      <c r="C18" s="56"/>
-      <c r="D18" s="56"/>
-      <c r="E18" t="s" s="117">
+      <c r="C18" s="46"/>
+      <c r="D18" s="46"/>
+      <c r="E18" t="s" s="106">
         <v>50</v>
       </c>
-      <c r="F18" t="s" s="117">
+      <c r="F18" t="s" s="106">
         <v>51</v>
       </c>
-      <c r="G18" s="58"/>
-      <c r="H18" s="58"/>
-      <c r="I18" s="59"/>
-      <c r="J18" t="s" s="117">
+      <c r="G18" s="48"/>
+      <c r="H18" s="48"/>
+      <c r="I18" s="49"/>
+      <c r="J18" t="s" s="106">
         <v>32</v>
       </c>
-      <c r="K18" t="s" s="117">
+      <c r="K18" t="s" s="106">
         <v>45</v>
       </c>
-      <c r="L18" t="s" s="117">
+      <c r="L18" t="s" s="106">
         <v>45</v>
       </c>
-      <c r="M18" t="s" s="117">
+      <c r="M18" t="s" s="106">
         <v>32</v>
       </c>
-      <c r="N18" s="28"/>
-      <c r="O18" s="29"/>
-      <c r="P18" s="28"/>
-      <c r="Q18" s="28"/>
-      <c r="R18" s="29"/>
-      <c r="S18" s="32"/>
-      <c r="T18" s="33"/>
+      <c r="N18" s="22"/>
+      <c r="O18" s="23"/>
+      <c r="P18" s="22"/>
+      <c r="Q18" s="22"/>
+      <c r="R18" s="23"/>
+      <c r="S18" s="26"/>
+      <c r="T18" s="27"/>
     </row>
-    <row r="19" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" t="n" s="117">
+    <row r="19" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" t="n" s="106">
         <v>4.0</v>
       </c>
-      <c r="B19" t="s" s="117">
+      <c r="B19" t="s" s="106">
         <v>52</v>
       </c>
-      <c r="C19" s="56"/>
-      <c r="D19" s="56"/>
-      <c r="E19" t="s" s="117">
+      <c r="C19" s="46"/>
+      <c r="D19" s="46"/>
+      <c r="E19" t="s" s="106">
         <v>53</v>
       </c>
-      <c r="F19" t="s" s="117">
+      <c r="F19" t="s" s="106">
         <v>54</v>
       </c>
-      <c r="G19" s="58"/>
-      <c r="H19" s="58"/>
-      <c r="I19" s="59"/>
-      <c r="J19" t="s" s="117">
+      <c r="G19" s="48"/>
+      <c r="H19" s="48"/>
+      <c r="I19" s="49"/>
+      <c r="J19" t="s" s="106">
         <v>32</v>
       </c>
-      <c r="K19" t="s" s="117">
+      <c r="K19" t="s" s="106">
         <v>45</v>
       </c>
-      <c r="L19" t="s" s="117">
+      <c r="L19" t="s" s="106">
         <v>45</v>
       </c>
-      <c r="M19" t="s" s="117">
+      <c r="M19" t="s" s="106">
         <v>32</v>
       </c>
-      <c r="N19" s="28"/>
-      <c r="O19" s="29"/>
-      <c r="P19" s="28"/>
-      <c r="Q19" s="28"/>
-      <c r="R19" s="29"/>
-      <c r="S19" s="32"/>
-      <c r="T19" s="33"/>
+      <c r="N19" s="22"/>
+      <c r="O19" s="23"/>
+      <c r="P19" s="22"/>
+      <c r="Q19" s="22"/>
+      <c r="R19" s="23"/>
+      <c r="S19" s="26"/>
+      <c r="T19" s="27"/>
     </row>
-    <row r="20" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" t="n" s="117">
+    <row r="20" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" t="n" s="106">
         <v>5.0</v>
       </c>
-      <c r="B20" t="s" s="117">
+      <c r="B20" t="s" s="106">
         <v>55</v>
       </c>
-      <c r="C20" s="56"/>
-      <c r="D20" s="56"/>
-      <c r="E20" t="s" s="117">
+      <c r="C20" s="46"/>
+      <c r="D20" s="46"/>
+      <c r="E20" t="s" s="106">
         <v>56</v>
       </c>
-      <c r="F20" t="s" s="117">
+      <c r="F20" t="s" s="106">
         <v>48</v>
       </c>
-      <c r="G20" s="58"/>
-      <c r="H20" s="58"/>
-      <c r="I20" s="59"/>
-      <c r="J20" t="s" s="117">
+      <c r="G20" s="48"/>
+      <c r="H20" s="48"/>
+      <c r="I20" s="49"/>
+      <c r="J20" t="s" s="106">
         <v>45</v>
       </c>
-      <c r="K20" t="s" s="117">
+      <c r="K20" t="s" s="106">
         <v>32</v>
       </c>
-      <c r="L20" t="s" s="117">
+      <c r="L20" t="s" s="106">
         <v>45</v>
       </c>
-      <c r="M20" t="s" s="117">
+      <c r="M20" t="s" s="106">
         <v>32</v>
       </c>
-      <c r="N20" s="28"/>
-      <c r="O20" s="29"/>
-      <c r="P20" s="28"/>
-      <c r="Q20" s="28"/>
-      <c r="R20" s="29"/>
-      <c r="S20" s="32"/>
-      <c r="T20" s="33"/>
+      <c r="N20" s="22"/>
+      <c r="O20" s="23"/>
+      <c r="P20" s="22"/>
+      <c r="Q20" s="22"/>
+      <c r="R20" s="23"/>
+      <c r="S20" s="26"/>
+      <c r="T20" s="27"/>
     </row>
-    <row r="21" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" t="n" s="117">
+    <row r="21" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" t="n" s="106">
         <v>6.0</v>
       </c>
-      <c r="B21" t="s" s="117">
+      <c r="B21" t="s" s="106">
         <v>57</v>
       </c>
-      <c r="C21" s="56"/>
-      <c r="D21" s="56"/>
-      <c r="E21" t="s" s="117">
+      <c r="C21" s="46"/>
+      <c r="D21" s="46"/>
+      <c r="E21" t="s" s="106">
         <v>58</v>
       </c>
-      <c r="F21" t="s" s="117">
+      <c r="F21" t="s" s="106">
         <v>44</v>
       </c>
-      <c r="G21" s="58"/>
-      <c r="H21" s="58"/>
-      <c r="I21" s="59"/>
-      <c r="J21" t="s" s="117">
+      <c r="G21" s="48"/>
+      <c r="H21" s="48"/>
+      <c r="I21" s="49"/>
+      <c r="J21" t="s" s="106">
         <v>32</v>
       </c>
-      <c r="K21" t="s" s="117">
+      <c r="K21" t="s" s="106">
         <v>45</v>
       </c>
-      <c r="L21" t="s" s="117">
+      <c r="L21" t="s" s="106">
         <v>32</v>
       </c>
-      <c r="M21" t="s" s="117">
+      <c r="M21" t="s" s="106">
         <v>45</v>
       </c>
-      <c r="N21" s="28"/>
-      <c r="O21" s="29"/>
-      <c r="P21" s="28"/>
-      <c r="Q21" s="28"/>
-      <c r="R21" s="29"/>
-      <c r="S21" s="32"/>
-      <c r="T21" s="33"/>
+      <c r="N21" s="22"/>
+      <c r="O21" s="23"/>
+      <c r="P21" s="22"/>
+      <c r="Q21" s="22"/>
+      <c r="R21" s="23"/>
+      <c r="S21" s="26"/>
+      <c r="T21" s="27"/>
     </row>
-    <row r="22" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="23"/>
-      <c r="B22" s="56"/>
-      <c r="C22" s="56"/>
-      <c r="D22" s="56"/>
-      <c r="E22" s="24"/>
-      <c r="F22" s="57"/>
-      <c r="G22" s="58"/>
-      <c r="H22" s="58"/>
-      <c r="I22" s="59"/>
-      <c r="J22" s="25"/>
-      <c r="K22" s="25"/>
-      <c r="L22" s="26"/>
-      <c r="M22" s="27"/>
-      <c r="N22" s="28"/>
-      <c r="O22" s="29"/>
-      <c r="P22" s="28"/>
-      <c r="Q22" s="28"/>
-      <c r="R22" s="29"/>
-      <c r="S22" s="32"/>
-      <c r="T22" s="33"/>
+    <row r="22" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="17"/>
+      <c r="B22" s="46"/>
+      <c r="C22" s="46"/>
+      <c r="D22" s="46"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="47"/>
+      <c r="G22" s="48"/>
+      <c r="H22" s="48"/>
+      <c r="I22" s="49"/>
+      <c r="J22" s="19"/>
+      <c r="K22" s="19"/>
+      <c r="L22" s="20"/>
+      <c r="M22" s="21"/>
+      <c r="N22" s="22"/>
+      <c r="O22" s="23"/>
+      <c r="P22" s="22"/>
+      <c r="Q22" s="22"/>
+      <c r="R22" s="23"/>
+      <c r="S22" s="26"/>
+      <c r="T22" s="27"/>
     </row>
-    <row r="23" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="23"/>
-      <c r="B23" s="56"/>
-      <c r="C23" s="56"/>
-      <c r="D23" s="56"/>
-      <c r="E23" s="24"/>
-      <c r="F23" s="57"/>
-      <c r="G23" s="58"/>
-      <c r="H23" s="58"/>
-      <c r="I23" s="59"/>
-      <c r="J23" s="25"/>
-      <c r="K23" s="25"/>
-      <c r="L23" s="26"/>
-      <c r="M23" s="27"/>
-      <c r="N23" s="28"/>
-      <c r="O23" s="29"/>
-      <c r="P23" s="28"/>
-      <c r="Q23" s="28"/>
-      <c r="R23" s="29"/>
-      <c r="S23" s="32"/>
-      <c r="T23" s="33"/>
+    <row r="23" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="17"/>
+      <c r="B23" s="46"/>
+      <c r="C23" s="46"/>
+      <c r="D23" s="46"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="47"/>
+      <c r="G23" s="48"/>
+      <c r="H23" s="48"/>
+      <c r="I23" s="49"/>
+      <c r="J23" s="19"/>
+      <c r="K23" s="19"/>
+      <c r="L23" s="20"/>
+      <c r="M23" s="21"/>
+      <c r="N23" s="22"/>
+      <c r="O23" s="23"/>
+      <c r="P23" s="22"/>
+      <c r="Q23" s="22"/>
+      <c r="R23" s="23"/>
+      <c r="S23" s="26"/>
+      <c r="T23" s="27"/>
     </row>
-    <row r="24" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="23"/>
-      <c r="B24" s="56"/>
-      <c r="C24" s="56"/>
-      <c r="D24" s="56"/>
-      <c r="E24" s="24"/>
-      <c r="F24" s="57"/>
-      <c r="G24" s="58"/>
-      <c r="H24" s="58"/>
-      <c r="I24" s="59"/>
-      <c r="J24" s="25"/>
-      <c r="K24" s="25"/>
-      <c r="L24" s="26"/>
-      <c r="M24" s="27"/>
-      <c r="N24" s="28"/>
-      <c r="O24" s="29"/>
-      <c r="P24" s="28"/>
-      <c r="Q24" s="28"/>
-      <c r="R24" s="29"/>
-      <c r="S24" s="32"/>
-      <c r="T24" s="33"/>
+    <row r="24" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="17"/>
+      <c r="B24" s="46"/>
+      <c r="C24" s="46"/>
+      <c r="D24" s="46"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="47"/>
+      <c r="G24" s="48"/>
+      <c r="H24" s="48"/>
+      <c r="I24" s="49"/>
+      <c r="J24" s="19"/>
+      <c r="K24" s="19"/>
+      <c r="L24" s="20"/>
+      <c r="M24" s="21"/>
+      <c r="N24" s="22"/>
+      <c r="O24" s="23"/>
+      <c r="P24" s="22"/>
+      <c r="Q24" s="22"/>
+      <c r="R24" s="23"/>
+      <c r="S24" s="26"/>
+      <c r="T24" s="27"/>
     </row>
-    <row r="25" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="23"/>
-      <c r="B25" s="56"/>
-      <c r="C25" s="56"/>
-      <c r="D25" s="56"/>
-      <c r="E25" s="24"/>
-      <c r="F25" s="57"/>
-      <c r="G25" s="58"/>
-      <c r="H25" s="58"/>
-      <c r="I25" s="59"/>
-      <c r="J25" s="25"/>
-      <c r="K25" s="25"/>
-      <c r="L25" s="26"/>
-      <c r="M25" s="27"/>
-      <c r="N25" s="28"/>
-      <c r="O25" s="29"/>
-      <c r="P25" s="28"/>
-      <c r="Q25" s="28"/>
-      <c r="R25" s="29"/>
-      <c r="S25" s="32"/>
-      <c r="T25" s="33"/>
+    <row r="25" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="17"/>
+      <c r="B25" s="46"/>
+      <c r="C25" s="46"/>
+      <c r="D25" s="46"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="47"/>
+      <c r="G25" s="48"/>
+      <c r="H25" s="48"/>
+      <c r="I25" s="49"/>
+      <c r="J25" s="19"/>
+      <c r="K25" s="19"/>
+      <c r="L25" s="20"/>
+      <c r="M25" s="21"/>
+      <c r="N25" s="22"/>
+      <c r="O25" s="23"/>
+      <c r="P25" s="22"/>
+      <c r="Q25" s="22"/>
+      <c r="R25" s="23"/>
+      <c r="S25" s="26"/>
+      <c r="T25" s="27"/>
     </row>
-    <row r="26" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="23"/>
-      <c r="B26" s="56"/>
-      <c r="C26" s="56"/>
-      <c r="D26" s="56"/>
-      <c r="E26" s="24"/>
-      <c r="F26" s="57"/>
-      <c r="G26" s="58"/>
-      <c r="H26" s="58"/>
-      <c r="I26" s="59"/>
-      <c r="J26" s="25"/>
-      <c r="K26" s="25"/>
-      <c r="L26" s="26"/>
-      <c r="M26" s="27"/>
-      <c r="N26" s="28"/>
-      <c r="O26" s="29"/>
-      <c r="P26" s="28"/>
-      <c r="Q26" s="28"/>
-      <c r="R26" s="29"/>
-      <c r="S26" s="32"/>
-      <c r="T26" s="33"/>
+    <row r="26" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="17"/>
+      <c r="B26" s="46"/>
+      <c r="C26" s="46"/>
+      <c r="D26" s="46"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="47"/>
+      <c r="G26" s="48"/>
+      <c r="H26" s="48"/>
+      <c r="I26" s="49"/>
+      <c r="J26" s="19"/>
+      <c r="K26" s="19"/>
+      <c r="L26" s="20"/>
+      <c r="M26" s="21"/>
+      <c r="N26" s="22"/>
+      <c r="O26" s="23"/>
+      <c r="P26" s="22"/>
+      <c r="Q26" s="22"/>
+      <c r="R26" s="23"/>
+      <c r="S26" s="26"/>
+      <c r="T26" s="27"/>
     </row>
-    <row r="27" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="23"/>
-      <c r="B27" s="56"/>
-      <c r="C27" s="56"/>
-      <c r="D27" s="56"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="57"/>
-      <c r="G27" s="58"/>
-      <c r="H27" s="58"/>
-      <c r="I27" s="59"/>
-      <c r="J27" s="25"/>
-      <c r="K27" s="25"/>
-      <c r="L27" s="26"/>
-      <c r="M27" s="27"/>
-      <c r="N27" s="28"/>
-      <c r="O27" s="29"/>
-      <c r="P27" s="28"/>
-      <c r="Q27" s="28"/>
-      <c r="R27" s="29"/>
-      <c r="S27" s="32"/>
-      <c r="T27" s="33"/>
+    <row r="27" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="17"/>
+      <c r="B27" s="46"/>
+      <c r="C27" s="46"/>
+      <c r="D27" s="46"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="47"/>
+      <c r="G27" s="48"/>
+      <c r="H27" s="48"/>
+      <c r="I27" s="49"/>
+      <c r="J27" s="19"/>
+      <c r="K27" s="19"/>
+      <c r="L27" s="20"/>
+      <c r="M27" s="21"/>
+      <c r="N27" s="22"/>
+      <c r="O27" s="23"/>
+      <c r="P27" s="22"/>
+      <c r="Q27" s="22"/>
+      <c r="R27" s="23"/>
+      <c r="S27" s="26"/>
+      <c r="T27" s="27"/>
     </row>
-    <row r="28" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="23"/>
-      <c r="B28" s="56"/>
-      <c r="C28" s="56"/>
-      <c r="D28" s="56"/>
-      <c r="E28" s="24"/>
-      <c r="F28" s="57"/>
-      <c r="G28" s="58"/>
-      <c r="H28" s="58"/>
-      <c r="I28" s="59"/>
-      <c r="J28" s="25"/>
-      <c r="K28" s="25"/>
-      <c r="L28" s="26"/>
-      <c r="M28" s="27"/>
-      <c r="N28" s="28"/>
-      <c r="O28" s="29"/>
-      <c r="P28" s="28"/>
-      <c r="Q28" s="28"/>
-      <c r="R28" s="29"/>
-      <c r="S28" s="32"/>
-      <c r="T28" s="33"/>
+    <row r="28" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="17"/>
+      <c r="B28" s="46"/>
+      <c r="C28" s="46"/>
+      <c r="D28" s="46"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="47"/>
+      <c r="G28" s="48"/>
+      <c r="H28" s="48"/>
+      <c r="I28" s="49"/>
+      <c r="J28" s="19"/>
+      <c r="K28" s="19"/>
+      <c r="L28" s="20"/>
+      <c r="M28" s="21"/>
+      <c r="N28" s="22"/>
+      <c r="O28" s="23"/>
+      <c r="P28" s="22"/>
+      <c r="Q28" s="22"/>
+      <c r="R28" s="23"/>
+      <c r="S28" s="26"/>
+      <c r="T28" s="27"/>
     </row>
-    <row r="29" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="23"/>
-      <c r="B29" s="56"/>
-      <c r="C29" s="56"/>
-      <c r="D29" s="56"/>
-      <c r="E29" s="24"/>
-      <c r="F29" s="57"/>
-      <c r="G29" s="58"/>
-      <c r="H29" s="58"/>
-      <c r="I29" s="59"/>
-      <c r="J29" s="25"/>
-      <c r="K29" s="25"/>
-      <c r="L29" s="26"/>
-      <c r="M29" s="27"/>
-      <c r="N29" s="28"/>
-      <c r="O29" s="29"/>
-      <c r="P29" s="28"/>
-      <c r="Q29" s="28"/>
-      <c r="R29" s="29"/>
-      <c r="S29" s="32"/>
-      <c r="T29" s="33"/>
+    <row r="29" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="17"/>
+      <c r="B29" s="46"/>
+      <c r="C29" s="46"/>
+      <c r="D29" s="46"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="47"/>
+      <c r="G29" s="48"/>
+      <c r="H29" s="48"/>
+      <c r="I29" s="49"/>
+      <c r="J29" s="19"/>
+      <c r="K29" s="19"/>
+      <c r="L29" s="20"/>
+      <c r="M29" s="21"/>
+      <c r="N29" s="22"/>
+      <c r="O29" s="23"/>
+      <c r="P29" s="22"/>
+      <c r="Q29" s="22"/>
+      <c r="R29" s="23"/>
+      <c r="S29" s="26"/>
+      <c r="T29" s="27"/>
     </row>
-    <row r="30" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="23"/>
-      <c r="B30" s="56"/>
-      <c r="C30" s="56"/>
-      <c r="D30" s="56"/>
-      <c r="E30" s="24"/>
-      <c r="F30" s="57"/>
-      <c r="G30" s="58"/>
-      <c r="H30" s="58"/>
-      <c r="I30" s="59"/>
-      <c r="J30" s="25"/>
-      <c r="K30" s="25"/>
-      <c r="L30" s="26"/>
-      <c r="M30" s="27"/>
-      <c r="N30" s="28"/>
-      <c r="O30" s="29"/>
-      <c r="P30" s="28"/>
-      <c r="Q30" s="28"/>
-      <c r="R30" s="29"/>
-      <c r="S30" s="32"/>
-      <c r="T30" s="33"/>
+    <row r="30" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="17"/>
+      <c r="B30" s="46"/>
+      <c r="C30" s="46"/>
+      <c r="D30" s="46"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="47"/>
+      <c r="G30" s="48"/>
+      <c r="H30" s="48"/>
+      <c r="I30" s="49"/>
+      <c r="J30" s="19"/>
+      <c r="K30" s="19"/>
+      <c r="L30" s="20"/>
+      <c r="M30" s="21"/>
+      <c r="N30" s="22"/>
+      <c r="O30" s="23"/>
+      <c r="P30" s="22"/>
+      <c r="Q30" s="22"/>
+      <c r="R30" s="23"/>
+      <c r="S30" s="26"/>
+      <c r="T30" s="27"/>
     </row>
-    <row r="31" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="23"/>
-      <c r="B31" s="56"/>
-      <c r="C31" s="56"/>
-      <c r="D31" s="56"/>
-      <c r="E31" s="24"/>
-      <c r="F31" s="57"/>
-      <c r="G31" s="58"/>
-      <c r="H31" s="58"/>
-      <c r="I31" s="59"/>
-      <c r="J31" s="25"/>
-      <c r="K31" s="25"/>
-      <c r="L31" s="26"/>
-      <c r="M31" s="27"/>
-      <c r="N31" s="28"/>
-      <c r="O31" s="29"/>
-      <c r="P31" s="28"/>
-      <c r="Q31" s="28"/>
-      <c r="R31" s="29"/>
-      <c r="S31" s="32"/>
-      <c r="T31" s="33"/>
+    <row r="31" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="17"/>
+      <c r="B31" s="46"/>
+      <c r="C31" s="46"/>
+      <c r="D31" s="46"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="47"/>
+      <c r="G31" s="48"/>
+      <c r="H31" s="48"/>
+      <c r="I31" s="49"/>
+      <c r="J31" s="19"/>
+      <c r="K31" s="19"/>
+      <c r="L31" s="20"/>
+      <c r="M31" s="21"/>
+      <c r="N31" s="22"/>
+      <c r="O31" s="23"/>
+      <c r="P31" s="22"/>
+      <c r="Q31" s="22"/>
+      <c r="R31" s="23"/>
+      <c r="S31" s="26"/>
+      <c r="T31" s="27"/>
     </row>
-    <row r="32" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="23"/>
-      <c r="B32" s="56"/>
-      <c r="C32" s="56"/>
-      <c r="D32" s="56"/>
-      <c r="E32" s="24"/>
-      <c r="F32" s="57"/>
-      <c r="G32" s="58"/>
-      <c r="H32" s="58"/>
-      <c r="I32" s="59"/>
-      <c r="J32" s="25"/>
-      <c r="K32" s="25"/>
-      <c r="L32" s="26"/>
-      <c r="M32" s="27"/>
-      <c r="N32" s="28"/>
-      <c r="O32" s="29"/>
-      <c r="P32" s="28"/>
-      <c r="Q32" s="28"/>
-      <c r="R32" s="29"/>
-      <c r="S32" s="32"/>
-      <c r="T32" s="33"/>
+    <row r="32" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="17"/>
+      <c r="B32" s="46"/>
+      <c r="C32" s="46"/>
+      <c r="D32" s="46"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="47"/>
+      <c r="G32" s="48"/>
+      <c r="H32" s="48"/>
+      <c r="I32" s="49"/>
+      <c r="J32" s="19"/>
+      <c r="K32" s="19"/>
+      <c r="L32" s="20"/>
+      <c r="M32" s="21"/>
+      <c r="N32" s="22"/>
+      <c r="O32" s="23"/>
+      <c r="P32" s="22"/>
+      <c r="Q32" s="22"/>
+      <c r="R32" s="23"/>
+      <c r="S32" s="26"/>
+      <c r="T32" s="27"/>
     </row>
-    <row r="33" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="23"/>
-      <c r="B33" s="56"/>
-      <c r="C33" s="56"/>
-      <c r="D33" s="56"/>
-      <c r="E33" s="24"/>
-      <c r="F33" s="57"/>
-      <c r="G33" s="58"/>
-      <c r="H33" s="58"/>
-      <c r="I33" s="59"/>
-      <c r="J33" s="25"/>
-      <c r="K33" s="25"/>
-      <c r="L33" s="26"/>
-      <c r="M33" s="27"/>
-      <c r="N33" s="28"/>
-      <c r="O33" s="29"/>
-      <c r="P33" s="28"/>
-      <c r="Q33" s="28"/>
-      <c r="R33" s="29"/>
-      <c r="S33" s="32"/>
-      <c r="T33" s="33"/>
+    <row r="33" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="17"/>
+      <c r="B33" s="46"/>
+      <c r="C33" s="46"/>
+      <c r="D33" s="46"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="47"/>
+      <c r="G33" s="48"/>
+      <c r="H33" s="48"/>
+      <c r="I33" s="49"/>
+      <c r="J33" s="19"/>
+      <c r="K33" s="19"/>
+      <c r="L33" s="20"/>
+      <c r="M33" s="21"/>
+      <c r="N33" s="22"/>
+      <c r="O33" s="23"/>
+      <c r="P33" s="22"/>
+      <c r="Q33" s="22"/>
+      <c r="R33" s="23"/>
+      <c r="S33" s="26"/>
+      <c r="T33" s="27"/>
     </row>
-    <row r="34" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="23"/>
-      <c r="B34" s="56"/>
-      <c r="C34" s="56"/>
-      <c r="D34" s="56"/>
-      <c r="E34" s="24"/>
-      <c r="F34" s="57"/>
-      <c r="G34" s="58"/>
-      <c r="H34" s="58"/>
-      <c r="I34" s="59"/>
-      <c r="J34" s="25"/>
-      <c r="K34" s="25"/>
-      <c r="L34" s="26"/>
-      <c r="M34" s="27"/>
-      <c r="N34" s="28"/>
-      <c r="O34" s="29"/>
-      <c r="P34" s="28"/>
-      <c r="Q34" s="28"/>
-      <c r="R34" s="29"/>
-      <c r="S34" s="32"/>
-      <c r="T34" s="33"/>
+    <row r="34" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="17"/>
+      <c r="B34" s="46"/>
+      <c r="C34" s="46"/>
+      <c r="D34" s="46"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="47"/>
+      <c r="G34" s="48"/>
+      <c r="H34" s="48"/>
+      <c r="I34" s="49"/>
+      <c r="J34" s="19"/>
+      <c r="K34" s="19"/>
+      <c r="L34" s="20"/>
+      <c r="M34" s="21"/>
+      <c r="N34" s="22"/>
+      <c r="O34" s="23"/>
+      <c r="P34" s="22"/>
+      <c r="Q34" s="22"/>
+      <c r="R34" s="23"/>
+      <c r="S34" s="26"/>
+      <c r="T34" s="27"/>
     </row>
-    <row r="35" spans="1:20" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="34"/>
-      <c r="B35" s="60"/>
-      <c r="C35" s="60"/>
-      <c r="D35" s="60"/>
-      <c r="E35" s="35"/>
-      <c r="F35" s="61"/>
-      <c r="G35" s="62"/>
-      <c r="H35" s="62"/>
-      <c r="I35" s="63"/>
-      <c r="J35" s="36"/>
-      <c r="K35" s="36"/>
-      <c r="L35" s="37"/>
-      <c r="M35" s="37"/>
-      <c r="N35" s="38"/>
-      <c r="O35" s="39"/>
-      <c r="P35" s="38"/>
-      <c r="Q35" s="38"/>
-      <c r="R35" s="39"/>
-      <c r="S35" s="40"/>
-      <c r="T35" s="41"/>
+    <row r="35" spans="1:20" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="28"/>
+      <c r="B35" s="50"/>
+      <c r="C35" s="50"/>
+      <c r="D35" s="50"/>
+      <c r="E35" s="29"/>
+      <c r="F35" s="51"/>
+      <c r="G35" s="52"/>
+      <c r="H35" s="52"/>
+      <c r="I35" s="53"/>
+      <c r="J35" s="30"/>
+      <c r="K35" s="30"/>
+      <c r="L35" s="31"/>
+      <c r="M35" s="31"/>
+      <c r="N35" s="32"/>
+      <c r="O35" s="33"/>
+      <c r="P35" s="32"/>
+      <c r="Q35" s="32"/>
+      <c r="R35" s="33"/>
+      <c r="S35" s="34"/>
+      <c r="T35" s="35"/>
     </row>
-    <row r="36" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="42" t="s">
+    <row r="36" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="B36" s="42"/>
-      <c r="C36" s="42"/>
-      <c r="D36" s="42"/>
-      <c r="E36" s="42"/>
-      <c r="F36" s="42"/>
-      <c r="G36" s="42"/>
-      <c r="H36" s="42"/>
-      <c r="I36" s="42"/>
-      <c r="J36" s="42"/>
-      <c r="K36" s="42"/>
-      <c r="L36" s="42"/>
-      <c r="M36" s="42"/>
-      <c r="N36" s="42"/>
-      <c r="O36" s="42"/>
-      <c r="P36" s="42"/>
-      <c r="Q36" s="42"/>
-      <c r="R36" s="42"/>
-      <c r="S36" s="43" t="s">
+      <c r="B36" s="36"/>
+      <c r="C36" s="36"/>
+      <c r="D36" s="36"/>
+      <c r="E36" s="36"/>
+      <c r="F36" s="36"/>
+      <c r="G36" s="36"/>
+      <c r="H36" s="36"/>
+      <c r="I36" s="36"/>
+      <c r="J36" s="36"/>
+      <c r="K36" s="36"/>
+      <c r="L36" s="36"/>
+      <c r="M36" s="36"/>
+      <c r="N36" s="36"/>
+      <c r="O36" s="36"/>
+      <c r="P36" s="36"/>
+      <c r="Q36" s="36"/>
+      <c r="R36" s="36"/>
+      <c r="S36" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="T36" s="3"/>
     </row>
-    <row r="37" spans="1:20" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="3"/>
-      <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="64"/>
-      <c r="E37" s="64"/>
-      <c r="F37" s="64"/>
-      <c r="G37" s="64"/>
-      <c r="H37" s="3"/>
-      <c r="I37" s="3"/>
-      <c r="J37" s="3"/>
-      <c r="K37" s="3"/>
-      <c r="L37" s="3"/>
-      <c r="M37" s="3"/>
-      <c r="N37" s="3"/>
-      <c r="O37" s="3"/>
-      <c r="P37" s="3"/>
-      <c r="Q37" s="3"/>
-      <c r="R37" s="3"/>
-      <c r="S37" s="3"/>
-      <c r="T37" s="3"/>
+    <row r="37" spans="1:20" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D37" s="54"/>
+      <c r="E37" s="54"/>
+      <c r="F37" s="54"/>
+      <c r="G37" s="54"/>
+      <c r="I37" s="43"/>
+      <c r="J37" s="43"/>
+      <c r="K37" s="43"/>
+      <c r="L37" s="43"/>
+      <c r="M37" s="43"/>
+      <c r="N37" s="43"/>
+      <c r="O37" s="43"/>
+      <c r="P37" s="43"/>
+      <c r="Q37" s="43"/>
+      <c r="R37" s="43"/>
+      <c r="S37" s="43"/>
+      <c r="T37" s="43"/>
     </row>
-    <row r="38" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="3"/>
-      <c r="B38" s="3"/>
-      <c r="C38" s="44"/>
-      <c r="D38" s="65" t="s">
+    <row r="38" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C38" s="38"/>
+      <c r="D38" s="99" t="s">
         <v>35</v>
       </c>
-      <c r="E38" s="65"/>
-      <c r="F38" s="65"/>
-      <c r="G38" s="65"/>
-      <c r="H38" s="3"/>
-      <c r="I38" s="66" t="s">
+      <c r="E38" s="99"/>
+      <c r="F38" s="99"/>
+      <c r="G38" s="99"/>
+      <c r="I38" s="100" t="s">
         <v>40</v>
       </c>
-      <c r="J38" s="66"/>
-      <c r="K38" s="66"/>
-      <c r="L38" s="66"/>
-      <c r="M38" s="66"/>
-      <c r="N38" s="66"/>
-      <c r="O38" s="66"/>
-      <c r="P38" s="66"/>
-      <c r="Q38" s="66"/>
-      <c r="R38" s="66"/>
-      <c r="S38" s="66"/>
-      <c r="T38" s="66"/>
+      <c r="J38" s="100"/>
+      <c r="K38" s="100"/>
+      <c r="L38" s="100"/>
+      <c r="M38" s="100"/>
+      <c r="N38" s="100"/>
+      <c r="O38" s="100"/>
+      <c r="P38" s="100"/>
+      <c r="Q38" s="100"/>
+      <c r="R38" s="100"/>
+      <c r="S38" s="100"/>
+      <c r="T38" s="100"/>
     </row>
-    <row r="39" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="3"/>
-      <c r="B39" s="3"/>
-      <c r="C39" s="3"/>
-      <c r="D39" s="49" t="s">
+    <row r="39" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D39" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="E39" s="49"/>
-      <c r="F39" s="49"/>
-      <c r="G39" s="49"/>
-      <c r="H39" s="3"/>
-      <c r="I39" s="50" t="s">
+      <c r="E39" s="40"/>
+      <c r="F39" s="40"/>
+      <c r="G39" s="40"/>
+      <c r="I39" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="J39" s="50"/>
-      <c r="K39" s="50"/>
-      <c r="L39" s="50"/>
-      <c r="M39" s="50"/>
-      <c r="N39" s="50"/>
-      <c r="O39" s="50"/>
-      <c r="P39" s="50"/>
-      <c r="Q39" s="50"/>
-      <c r="R39" s="50"/>
-      <c r="S39" s="50"/>
-      <c r="T39" s="50"/>
+      <c r="J39" s="41"/>
+      <c r="K39" s="41"/>
+      <c r="L39" s="41"/>
+      <c r="M39" s="41"/>
+      <c r="N39" s="41"/>
+      <c r="O39" s="41"/>
+      <c r="P39" s="41"/>
+      <c r="Q39" s="41"/>
+      <c r="R39" s="41"/>
+      <c r="S39" s="41"/>
+      <c r="T39" s="41"/>
     </row>
-    <row r="40" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="3"/>
-      <c r="B40" s="3"/>
-      <c r="C40" s="3"/>
-      <c r="D40" s="51"/>
-      <c r="E40" s="51"/>
-      <c r="F40" s="51"/>
-      <c r="G40" s="51"/>
-      <c r="H40" s="3"/>
-      <c r="I40" s="52" t="s">
+    <row r="40" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D40" s="42"/>
+      <c r="E40" s="42"/>
+      <c r="F40" s="42"/>
+      <c r="G40" s="42"/>
+      <c r="I40" s="43" t="s">
         <v>31</v>
       </c>
-      <c r="J40" s="52"/>
-      <c r="K40" s="52"/>
-      <c r="L40" s="52"/>
-      <c r="M40" s="52"/>
-      <c r="N40" s="52"/>
-      <c r="O40" s="52"/>
-      <c r="P40" s="52"/>
-      <c r="Q40" s="52"/>
-      <c r="R40" s="52"/>
-      <c r="S40" s="52"/>
-      <c r="T40" s="52"/>
+      <c r="J40" s="43"/>
+      <c r="K40" s="43"/>
+      <c r="L40" s="43"/>
+      <c r="M40" s="43"/>
+      <c r="N40" s="43"/>
+      <c r="O40" s="43"/>
+      <c r="P40" s="43"/>
+      <c r="Q40" s="43"/>
+      <c r="R40" s="43"/>
+      <c r="S40" s="43"/>
+      <c r="T40" s="43"/>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A41" s="3"/>
-      <c r="B41" s="3"/>
-      <c r="C41" s="3"/>
-      <c r="D41" s="51"/>
-      <c r="E41" s="51"/>
-      <c r="F41" s="51"/>
-      <c r="G41" s="51"/>
-      <c r="H41" s="3"/>
-      <c r="I41" s="3"/>
-      <c r="J41" s="3"/>
-      <c r="K41" s="3"/>
-      <c r="L41" s="3"/>
-      <c r="M41" s="3"/>
-      <c r="N41" s="3"/>
-      <c r="O41" s="3"/>
-      <c r="P41" s="3"/>
-      <c r="Q41" s="3"/>
-      <c r="R41" s="3"/>
-      <c r="S41" s="3"/>
-      <c r="T41" s="3"/>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="D41" s="42"/>
+      <c r="E41" s="42"/>
+      <c r="F41" s="42"/>
+      <c r="G41" s="42"/>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A42" s="53"/>
-      <c r="B42" s="53"/>
-      <c r="C42" s="53"/>
-      <c r="D42" s="53"/>
-      <c r="E42" s="53"/>
-      <c r="F42" s="53"/>
-      <c r="G42" s="53"/>
-      <c r="H42" s="53"/>
-      <c r="T42" s="45"/>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A42" s="44"/>
+      <c r="B42" s="44"/>
+      <c r="C42" s="44"/>
+      <c r="D42" s="44"/>
+      <c r="E42" s="44"/>
+      <c r="F42" s="44"/>
+      <c r="G42" s="44"/>
+      <c r="H42" s="44"/>
+      <c r="T42" s="39"/>
     </row>
   </sheetData>
-  <mergeCells count="75">
+  <mergeCells count="78">
     <mergeCell ref="B6:R6"/>
     <mergeCell ref="D8:S8"/>
     <mergeCell ref="A9:C9"/>
@@ -5011,6 +4929,7 @@
     <mergeCell ref="B13:D15"/>
     <mergeCell ref="E13:E15"/>
     <mergeCell ref="F13:I15"/>
+    <mergeCell ref="D11:H11"/>
     <mergeCell ref="J13:J15"/>
     <mergeCell ref="K13:K15"/>
     <mergeCell ref="L13:M13"/>
@@ -5037,7 +4956,6 @@
     <mergeCell ref="F23:I23"/>
     <mergeCell ref="B24:D24"/>
     <mergeCell ref="F24:I24"/>
-    <mergeCell ref="D37:G38"/>
     <mergeCell ref="I38:T38"/>
     <mergeCell ref="B31:D31"/>
     <mergeCell ref="F31:I31"/>
@@ -5045,6 +4963,9 @@
     <mergeCell ref="F32:I32"/>
     <mergeCell ref="B33:D33"/>
     <mergeCell ref="F33:I33"/>
+    <mergeCell ref="D37:G37"/>
+    <mergeCell ref="I37:T37"/>
+    <mergeCell ref="D38:G38"/>
     <mergeCell ref="K10:R10"/>
     <mergeCell ref="K11:R11"/>
     <mergeCell ref="B34:D34"/>
@@ -5067,37 +4988,27 @@
     <mergeCell ref="I40:T40"/>
     <mergeCell ref="A42:H42"/>
   </mergeCells>
-  <conditionalFormatting sqref="E16:E35">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+  <conditionalFormatting sqref="A16:R35">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D40">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N16:R35">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="T1:T8 T36:T1048576 T10:T15">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+  <conditionalFormatting sqref="T1:T8 T10:T15 T36 T39:T1048576">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>50</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A16:R35">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="¡¡¡CUIDADO!!!" error="...Tiene fórmula. Solo puede modificar en la bd PARTICIPANTES" sqref="A16:K35"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="¡¡¡CUIDADO!!!" error="...Tiene fórmula. Solo puede modificar en la bd PARTICIPANTES" sqref="A16:K35" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
   </dataValidations>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
-  <pageSetup scale="79" orientation="landscape" r:id="rId1"/>
+  <pageSetup scale="82" orientation="landscape" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddFooter>&amp;R&amp;6CÓDIGO 711-DP-PO-005-019-A2</oddFooter>
   </headerFooter>

</xml_diff>